<commit_message>
in sale sch not added data done that
</commit_message>
<xml_diff>
--- a/eTactWeb/wwwroot/Uploads/ImportDayWiseFormat (1).xlsx
+++ b/eTactWeb/wwwroot/Uploads/ImportDayWiseFormat (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D43459A5-41D6-4870-BD30-7A77BC4F5808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87D6143-F0D7-408A-96B1-E5E7B97A9D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="20376" windowHeight="12096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Part Code</t>
   </si>
@@ -115,14 +115,23 @@
     <t>30</t>
   </si>
   <si>
-    <t>FGFG00004</t>
+    <t>5164LM-665</t>
+  </si>
+  <si>
+    <t>5164L-665</t>
+  </si>
+  <si>
+    <t>6171B-617</t>
+  </si>
+  <si>
+    <t>5114P-665</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -136,6 +145,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFFF0000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -164,9 +179,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,15 +523,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AE5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -609,7 +626,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -623,9 +640,57 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="15.6" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>22</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4">
+        <v>400</v>
+      </c>
+      <c r="F4">
+        <v>777</v>
+      </c>
+      <c r="H4">
+        <v>100</v>
+      </c>
+      <c r="J4">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5">
+        <v>233</v>
+      </c>
+      <c r="D5">
+        <v>444</v>
+      </c>
+      <c r="G5">
+        <v>332</v>
+      </c>
+      <c r="I5">
+        <v>2222</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="A1:AE1" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>